<commit_message>
Added spell cooldown meters and cooldownlist
Added CooldownList object that manages a set of BarMeter objects (I did a Unity). Maximum 6 spells can be cooling. List collapses when a spell finishes. CooldownList now handles spell cooldown timers (not Timer.cs). removed Timer object from scene,  as it is not being used. Added two new root keywords (spear and falchion) for testing purposes
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/spellDictionary.xlsx
+++ b/Typocrypha/Assets/spellDictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>name (root)</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>aimed</t>
+  </si>
+  <si>
+    <t>spear</t>
+  </si>
+  <si>
+    <t>a basic long cool atk</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,37 +483,52 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>90</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -515,10 +536,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -526,48 +547,59 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10">
-        <v>-5</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="E10">
-        <v>0</v>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>-5</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>